<commit_message>
Simple Knolls working Spawning working Doors between wells are in
</commit_message>
<xml_diff>
--- a/notes/WellThoughts.xlsx
+++ b/notes/WellThoughts.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="16260" windowHeight="9000"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="16260" windowHeight="9000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Oddz" sheetId="1" r:id="rId1"/>
     <sheet name="Wall" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Doors" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>w-1</t>
   </si>
@@ -121,7 +121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +131,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
@@ -378,13 +390,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" textRotation="180" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
@@ -704,10 +731,10 @@
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="26"/>
+      <c r="Q1" s="27"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -784,7 +811,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="10"/>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="28" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="1">
@@ -814,7 +841,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="10"/>
-      <c r="L6" s="27"/>
+      <c r="L6" s="28"/>
       <c r="O6" s="6"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="9"/>
@@ -1200,542 +1227,542 @@
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B1" s="28"/>
-      <c r="Q1" s="28"/>
+      <c r="B1" s="26"/>
+      <c r="Q1" s="26"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B2" s="28"/>
-      <c r="Q2" s="28"/>
+      <c r="B2" s="26"/>
+      <c r="Q2" s="26"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
+      <c r="B3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
+      <c r="B4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="S5" s="28"/>
+      <c r="B5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="S5" s="26"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="S6" s="28"/>
+      <c r="B6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="S6" s="26"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="T7" s="28"/>
+      <c r="B7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="T7" s="26"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="T8" s="28"/>
+      <c r="B8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="T8" s="26"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="U9" s="28"/>
+      <c r="B9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="U9" s="26"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="U10" s="28"/>
+      <c r="B10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="U10" s="26"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="V11" s="28"/>
+      <c r="B11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="V11" s="26"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="V12" s="28"/>
+      <c r="B12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="V12" s="26"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="W13" s="28"/>
+      <c r="B13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="W13" s="26"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="W14" s="28"/>
+      <c r="B14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="W14" s="26"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="X15" s="28"/>
+      <c r="B15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="X15" s="26"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
-      <c r="V16" s="28"/>
-      <c r="W16" s="28"/>
-      <c r="X16" s="28"/>
+      <c r="B16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="26"/>
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="26"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="28"/>
-      <c r="D33" s="28"/>
+      <c r="B33" s="26"/>
+      <c r="D33" s="26"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="28"/>
-      <c r="D34" s="28"/>
+      <c r="B34" s="26"/>
+      <c r="D34" s="26"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="28"/>
-      <c r="D35" s="28"/>
+      <c r="B35" s="26"/>
+      <c r="D35" s="26"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="28"/>
-      <c r="D36" s="28"/>
+      <c r="B36" s="26"/>
+      <c r="D36" s="26"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="28"/>
-      <c r="D37" s="28"/>
+      <c r="B37" s="26"/>
+      <c r="D37" s="26"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="28"/>
-      <c r="D38" s="28"/>
+      <c r="B38" s="26"/>
+      <c r="D38" s="26"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="28"/>
-      <c r="D39" s="28"/>
+      <c r="B39" s="26"/>
+      <c r="D39" s="26"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="28"/>
-      <c r="D40" s="28"/>
+      <c r="B40" s="26"/>
+      <c r="D40" s="26"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="28"/>
-      <c r="D41" s="28"/>
+      <c r="B41" s="26"/>
+      <c r="D41" s="26"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="28"/>
-      <c r="D42" s="28"/>
+      <c r="B42" s="26"/>
+      <c r="D42" s="26"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="28"/>
-      <c r="D43" s="28"/>
+      <c r="B43" s="26"/>
+      <c r="D43" s="26"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="28"/>
-      <c r="D44" s="28"/>
+      <c r="B44" s="26"/>
+      <c r="D44" s="26"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="28"/>
-      <c r="D45" s="28"/>
+      <c r="B45" s="26"/>
+      <c r="D45" s="26"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="28"/>
-      <c r="D46" s="28"/>
+      <c r="B46" s="26"/>
+      <c r="D46" s="26"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="28"/>
-      <c r="D47" s="28"/>
+      <c r="B47" s="26"/>
+      <c r="D47" s="26"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="28"/>
-      <c r="D48" s="28"/>
+      <c r="B48" s="26"/>
+      <c r="D48" s="26"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="28"/>
-      <c r="E49" s="28"/>
+      <c r="B49" s="26"/>
+      <c r="E49" s="26"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="28"/>
-      <c r="E50" s="28"/>
+      <c r="B50" s="26"/>
+      <c r="E50" s="26"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="28"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="26"/>
+      <c r="E51" s="26"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="28"/>
-      <c r="E52" s="28"/>
+      <c r="B52" s="26"/>
+      <c r="E52" s="26"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="28"/>
-      <c r="E53" s="28"/>
+      <c r="B53" s="26"/>
+      <c r="E53" s="26"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="28"/>
-      <c r="E54" s="28"/>
+      <c r="B54" s="26"/>
+      <c r="E54" s="26"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="28"/>
-      <c r="E55" s="28"/>
+      <c r="B55" s="26"/>
+      <c r="E55" s="26"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="28"/>
-      <c r="E56" s="28"/>
+      <c r="B56" s="26"/>
+      <c r="E56" s="26"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="28"/>
-      <c r="E57" s="28"/>
+      <c r="B57" s="26"/>
+      <c r="E57" s="26"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="28"/>
-      <c r="E58" s="28"/>
+      <c r="B58" s="26"/>
+      <c r="E58" s="26"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="28"/>
-      <c r="E59" s="28"/>
+      <c r="B59" s="26"/>
+      <c r="E59" s="26"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="28"/>
-      <c r="E60" s="28"/>
+      <c r="B60" s="26"/>
+      <c r="E60" s="26"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="28"/>
-      <c r="E61" s="28"/>
+      <c r="B61" s="26"/>
+      <c r="E61" s="26"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="28"/>
-      <c r="E62" s="28"/>
+      <c r="B62" s="26"/>
+      <c r="E62" s="26"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="28"/>
-      <c r="E63" s="28"/>
+      <c r="B63" s="26"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B64" s="28"/>
-      <c r="E64" s="28"/>
+      <c r="B64" s="26"/>
+      <c r="E64" s="26"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B65" s="28"/>
-      <c r="F65" s="28"/>
+      <c r="B65" s="26"/>
+      <c r="F65" s="26"/>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B66" s="28"/>
-      <c r="F66" s="28"/>
+      <c r="B66" s="26"/>
+      <c r="F66" s="26"/>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B67" s="28"/>
-      <c r="F67" s="28"/>
+      <c r="B67" s="26"/>
+      <c r="F67" s="26"/>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B68" s="28"/>
-      <c r="F68" s="28"/>
+      <c r="B68" s="26"/>
+      <c r="F68" s="26"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B69" s="28"/>
-      <c r="F69" s="28"/>
+      <c r="B69" s="26"/>
+      <c r="F69" s="26"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B70" s="28"/>
-      <c r="F70" s="28"/>
+      <c r="B70" s="26"/>
+      <c r="F70" s="26"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B71" s="28"/>
-      <c r="F71" s="28"/>
+      <c r="B71" s="26"/>
+      <c r="F71" s="26"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B72" s="28"/>
-      <c r="F72" s="28"/>
+      <c r="B72" s="26"/>
+      <c r="F72" s="26"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B73" s="28"/>
-      <c r="F73" s="28"/>
+      <c r="B73" s="26"/>
+      <c r="F73" s="26"/>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B74" s="28"/>
-      <c r="F74" s="28"/>
+      <c r="B74" s="26"/>
+      <c r="F74" s="26"/>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B75" s="28"/>
-      <c r="F75" s="28"/>
+      <c r="B75" s="26"/>
+      <c r="F75" s="26"/>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B76" s="28"/>
-      <c r="F76" s="28"/>
+      <c r="B76" s="26"/>
+      <c r="F76" s="26"/>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B77" s="28"/>
-      <c r="F77" s="28"/>
+      <c r="B77" s="26"/>
+      <c r="F77" s="26"/>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B78" s="28"/>
-      <c r="F78" s="28"/>
+      <c r="B78" s="26"/>
+      <c r="F78" s="26"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B79" s="28"/>
-      <c r="F79" s="28"/>
+      <c r="B79" s="26"/>
+      <c r="F79" s="26"/>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B80" s="28"/>
-      <c r="F80" s="28"/>
+      <c r="B80" s="26"/>
+      <c r="F80" s="26"/>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B81" s="28"/>
-      <c r="G81" s="28"/>
+      <c r="B81" s="26"/>
+      <c r="G81" s="26"/>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B82" s="28"/>
-      <c r="G82" s="28"/>
+      <c r="B82" s="26"/>
+      <c r="G82" s="26"/>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B83" s="28"/>
-      <c r="G83" s="28"/>
+      <c r="B83" s="26"/>
+      <c r="G83" s="26"/>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B84" s="28"/>
-      <c r="G84" s="28"/>
+      <c r="B84" s="26"/>
+      <c r="G84" s="26"/>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B85" s="28"/>
-      <c r="G85" s="28"/>
+      <c r="B85" s="26"/>
+      <c r="G85" s="26"/>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B86" s="28"/>
-      <c r="G86" s="28"/>
+      <c r="B86" s="26"/>
+      <c r="G86" s="26"/>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B87" s="28"/>
-      <c r="G87" s="28"/>
+      <c r="B87" s="26"/>
+      <c r="G87" s="26"/>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B88" s="28"/>
-      <c r="G88" s="28"/>
+      <c r="B88" s="26"/>
+      <c r="G88" s="26"/>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B89" s="28"/>
-      <c r="G89" s="28"/>
+      <c r="B89" s="26"/>
+      <c r="G89" s="26"/>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B90" s="28"/>
-      <c r="G90" s="28"/>
+      <c r="B90" s="26"/>
+      <c r="G90" s="26"/>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B91" s="28"/>
-      <c r="G91" s="28"/>
+      <c r="B91" s="26"/>
+      <c r="G91" s="26"/>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B92" s="28"/>
-      <c r="G92" s="28"/>
+      <c r="B92" s="26"/>
+      <c r="G92" s="26"/>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B93" s="28"/>
-      <c r="G93" s="28"/>
+      <c r="B93" s="26"/>
+      <c r="G93" s="26"/>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B94" s="28"/>
-      <c r="G94" s="28"/>
+      <c r="B94" s="26"/>
+      <c r="G94" s="26"/>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B95" s="28"/>
-      <c r="G95" s="28"/>
+      <c r="B95" s="26"/>
+      <c r="G95" s="26"/>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B96" s="28"/>
-      <c r="G96" s="28"/>
+      <c r="B96" s="26"/>
+      <c r="G96" s="26"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B97" s="28"/>
-      <c r="H97" s="28"/>
+      <c r="B97" s="26"/>
+      <c r="H97" s="26"/>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B98" s="28"/>
-      <c r="H98" s="28"/>
+      <c r="B98" s="26"/>
+      <c r="H98" s="26"/>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B99" s="28"/>
-      <c r="H99" s="28"/>
+      <c r="B99" s="26"/>
+      <c r="H99" s="26"/>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B100" s="28"/>
-      <c r="H100" s="28"/>
+      <c r="B100" s="26"/>
+      <c r="H100" s="26"/>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B101" s="28"/>
-      <c r="H101" s="28"/>
+      <c r="B101" s="26"/>
+      <c r="H101" s="26"/>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B102" s="28"/>
-      <c r="H102" s="28"/>
+      <c r="B102" s="26"/>
+      <c r="H102" s="26"/>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B103" s="28"/>
-      <c r="H103" s="28"/>
+      <c r="B103" s="26"/>
+      <c r="H103" s="26"/>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B104" s="28"/>
-      <c r="H104" s="28"/>
+      <c r="B104" s="26"/>
+      <c r="H104" s="26"/>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B105" s="28"/>
-      <c r="H105" s="28"/>
+      <c r="B105" s="26"/>
+      <c r="H105" s="26"/>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B106" s="28"/>
-      <c r="H106" s="28"/>
+      <c r="B106" s="26"/>
+      <c r="H106" s="26"/>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B107" s="28"/>
-      <c r="H107" s="28"/>
+      <c r="B107" s="26"/>
+      <c r="H107" s="26"/>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B108" s="28"/>
-      <c r="H108" s="28"/>
+      <c r="B108" s="26"/>
+      <c r="H108" s="26"/>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B109" s="28"/>
-      <c r="H109" s="28"/>
+      <c r="B109" s="26"/>
+      <c r="H109" s="26"/>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B110" s="28"/>
-      <c r="H110" s="28"/>
+      <c r="B110" s="26"/>
+      <c r="H110" s="26"/>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B111" s="28"/>
-      <c r="H111" s="28"/>
+      <c r="B111" s="26"/>
+      <c r="H111" s="26"/>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B112" s="28"/>
-      <c r="H112" s="28"/>
+      <c r="B112" s="26"/>
+      <c r="H112" s="26"/>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B113" s="28"/>
-      <c r="I113" s="28"/>
+      <c r="B113" s="26"/>
+      <c r="I113" s="26"/>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B114" s="28"/>
-      <c r="I114" s="28"/>
+      <c r="B114" s="26"/>
+      <c r="I114" s="26"/>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B115" s="28"/>
-      <c r="I115" s="28"/>
+      <c r="B115" s="26"/>
+      <c r="I115" s="26"/>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B116" s="28"/>
-      <c r="I116" s="28"/>
+      <c r="B116" s="26"/>
+      <c r="I116" s="26"/>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B117" s="28"/>
-      <c r="I117" s="28"/>
+      <c r="B117" s="26"/>
+      <c r="I117" s="26"/>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B118" s="28"/>
-      <c r="I118" s="28"/>
+      <c r="B118" s="26"/>
+      <c r="I118" s="26"/>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B119" s="28"/>
-      <c r="I119" s="28"/>
+      <c r="B119" s="26"/>
+      <c r="I119" s="26"/>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B120" s="28"/>
-      <c r="I120" s="28"/>
+      <c r="B120" s="26"/>
+      <c r="I120" s="26"/>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B121" s="28"/>
-      <c r="I121" s="28"/>
+      <c r="B121" s="26"/>
+      <c r="I121" s="26"/>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B122" s="28"/>
-      <c r="I122" s="28"/>
+      <c r="B122" s="26"/>
+      <c r="I122" s="26"/>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B123" s="28"/>
-      <c r="I123" s="28"/>
+      <c r="B123" s="26"/>
+      <c r="I123" s="26"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B124" s="28"/>
-      <c r="I124" s="28"/>
+      <c r="B124" s="26"/>
+      <c r="I124" s="26"/>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B125" s="28"/>
-      <c r="I125" s="28"/>
+      <c r="B125" s="26"/>
+      <c r="I125" s="26"/>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B126" s="28"/>
-      <c r="I126" s="28"/>
+      <c r="B126" s="26"/>
+      <c r="I126" s="26"/>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B127" s="28"/>
-      <c r="I127" s="28"/>
+      <c r="B127" s="26"/>
+      <c r="I127" s="26"/>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B128" s="28"/>
-      <c r="C128" s="28"/>
-      <c r="D128" s="28"/>
-      <c r="E128" s="28"/>
-      <c r="F128" s="28"/>
-      <c r="G128" s="28"/>
-      <c r="H128" s="28"/>
-      <c r="I128" s="28"/>
+      <c r="B128" s="26"/>
+      <c r="C128" s="26"/>
+      <c r="D128" s="26"/>
+      <c r="E128" s="26"/>
+      <c r="F128" s="26"/>
+      <c r="G128" s="26"/>
+      <c r="H128" s="26"/>
+      <c r="I128" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1744,12 +1771,519 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <f>+B1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <f t="shared" ref="D1:Q1" si="0">+C1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A17" si="1">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="32"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
+      <c r="V13" s="29"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="33"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="33"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with the latest pushed to DevBukkit
</commit_message>
<xml_diff>
--- a/notes/WellThoughts.xlsx
+++ b/notes/WellThoughts.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="16260" windowHeight="9000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="16260" windowHeight="9000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Oddz" sheetId="1" r:id="rId1"/>
     <sheet name="Wall" sheetId="2" r:id="rId2"/>
     <sheet name="Doors" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -121,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +147,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -313,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
@@ -406,13 +431,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" textRotation="180" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,10 +776,10 @@
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="42"/>
+      <c r="Q1" s="43"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -812,7 +856,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="10"/>
-      <c r="L5" s="43" t="s">
+      <c r="L5" s="44" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="1">
@@ -842,7 +886,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="10"/>
-      <c r="L6" s="43"/>
+      <c r="L6" s="44"/>
       <c r="O6" s="6"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="9"/>
@@ -1774,7 +1818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z11" sqref="Z11:Z12"/>
     </sheetView>
   </sheetViews>
@@ -1914,9 +1958,9 @@
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
       <c r="I4" s="27"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="27"/>
       <c r="N4" s="27"/>
       <c r="O4" s="27"/>
@@ -2000,7 +2044,7 @@
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
-      <c r="O7" s="44"/>
+      <c r="O7" s="42"/>
       <c r="P7" s="31"/>
       <c r="Q7" s="34"/>
       <c r="R7" s="30"/>
@@ -2027,7 +2071,7 @@
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
-      <c r="O8" s="44"/>
+      <c r="O8" s="42"/>
       <c r="P8" s="38"/>
       <c r="Q8" s="39"/>
       <c r="R8" s="30"/>
@@ -2054,7 +2098,7 @@
       <c r="L9" s="27"/>
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
-      <c r="O9" s="44"/>
+      <c r="O9" s="42"/>
       <c r="P9" s="31"/>
       <c r="Q9" s="39"/>
       <c r="R9" s="37"/>
@@ -2070,7 +2114,7 @@
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="31"/>
-      <c r="D10" s="44"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
@@ -2097,7 +2141,7 @@
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="38"/>
-      <c r="D11" s="44"/>
+      <c r="D11" s="42"/>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
@@ -2124,7 +2168,7 @@
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="31"/>
-      <c r="D12" s="44"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
@@ -2208,9 +2252,9 @@
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
@@ -2287,4 +2331,307 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:Q17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="47"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B3" s="48"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="49"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="56"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="49"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B5" s="48"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="49"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="48"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="49"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="48"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="49"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="48"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="49"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="48"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="49"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="48"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="49"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B11" s="48"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="49"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="48"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="49"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="48"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="49"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="60"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="49"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="60"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="62"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="60"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="49"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="50"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="52"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Made Platform more random Shift every other row to make the wells more "hexagonal-ish"
</commit_message>
<xml_diff>
--- a/notes/WellThoughts.xlsx
+++ b/notes/WellThoughts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="16260" windowHeight="9000" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="16260" windowHeight="9000" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Oddz" sheetId="1" r:id="rId1"/>
@@ -17,19 +17,22 @@
     <sheet name="Calculations" sheetId="7" r:id="rId8"/>
     <sheet name="Hex step" sheetId="9" r:id="rId9"/>
     <sheet name="VolcanoShape" sheetId="10" r:id="rId10"/>
+    <sheet name="HexCalc2" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet2" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="HalfPi">VolcanoShape!$F$2</definedName>
     <definedName name="Steps">VolcanoShape!$G$1</definedName>
     <definedName name="TwoPi">VolcanoShape!$F$1</definedName>
     <definedName name="WellWidth">'Hex step'!$A$1</definedName>
+    <definedName name="WellWidth2">HexCalc2!$B$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
   <si>
     <t>w-1</t>
   </si>
@@ -120,18 +123,132 @@
   <si>
     <t>(i+1)* 16</t>
   </si>
+  <si>
+    <t>ChunkLocation comes in</t>
+  </si>
+  <si>
+    <t>Find the Chunk's Well Origin</t>
+  </si>
+  <si>
+    <t>Calculate the well origin location</t>
+  </si>
+  <si>
+    <t>If there is a well already defined</t>
+  </si>
+  <si>
+    <t>return it</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>create it</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = -8 Zs =  (-8)-8 (-8)-7 (-8)-6 (-8)-5 (-4)-4 (-4)-3 (-4)-2 (-4)-1 (0)0 (0)1 (0)2 (0)3 (4)4 (4)5 (4)6 (4)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = -7 Zs =  (-8)-8 (-8)-7 (-8)-6 (-8)-5 (-4)-4 (-4)-3 (-4)-2 (-4)-1 (0)0 (0)1 (0)2 (0)3 (4)4 (4)5 (4)6 (4)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = -6 Zs =  (-8)-8 (-8)-7 (-8)-6 (-8)-5 (-4)-4 (-4)-3 (-4)-2 (-4)-1 (0)0 (0)1 (0)2 (0)3 (4)4 (4)5 (4)6 (4)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = -5 Zs =  (-8)-8 (-8)-7 (-8)-6 (-8)-5 (-4)-4 (-4)-3 (-4)-2 (-4)-1 (0)0 (0)1 (0)2 (0)3 (4)4 (4)5 (4)6 (4)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = -4 Zs =  (-6)-8 (-6)-7 (-6)-6 (-6)-5 (-2)-4 (-2)-3 (-2)-2 (-2)-1 (2)0 (2)1 (2)2 (2)3 (6)4 (6)5 (6)6 (6)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = -3 Zs =  (-6)-8 (-6)-7 (-6)-6 (-6)-5 (-2)-4 (-2)-3 (-2)-2 (-2)-1 (2)0 (2)1 (2)2 (2)3 (6)4 (6)5 (6)6 (6)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = -2 Zs =  (-6)-8 (-6)-7 (-6)-6 (-6)-5 (-2)-4 (-2)-3 (-2)-2 (-2)-1 (2)0 (2)1 (2)2 (2)3 (6)4 (6)5 (6)6 (6)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = -1 Zs =  (-6)-8 (-6)-7 (-6)-6 (-6)-5 (-2)-4 (-2)-3 (-2)-2 (-2)-1 (2)0 (2)1 (2)2 (2)3 (6)4 (6)5 (6)6 (6)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = 0 Zs =   (-8)-8 (-8)-7 (-8)-6 (-8)-5 (-4)-4 (-4)-3 (-4)-2 (-4)-1 (0)0 (0)1 (0)2 (0)3 (4)4 (4)5 (4)6 (4)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = 1 Zs =   (-8)-8 (-8)-7 (-8)-6 (-8)-5 (-4)-4 (-4)-3 (-4)-2 (-4)-1 (0)0 (0)1 (0)2 (0)3 (4)4 (4)5 (4)6 (4)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = 2 Zs =   (-8)-8 (-8)-7 (-8)-6 (-8)-5 (-4)-4 (-4)-3 (-4)-2 (-4)-1 (0)0 (0)1 (0)2 (0)3 (4)4 (4)5 (4)6 (4)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = 3 Zs =   (-8)-8 (-8)-7 (-8)-6 (-8)-5 (-4)-4 (-4)-3 (-4)-2 (-4)-1 (0)0 (0)1 (0)2 (0)3 (4)4 (4)5 (4)6 (4)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = 4 Zs =   (-6)-8 (-6)-7 (-6)-6 (-6)-5 (-2)-4 (-2)-3 (-2)-2 (-2)-1 (2)0 (2)1 (2)2 (2)3 (6)4 (6)5 (6)6 (6)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = 5 Zs =   (-6)-8 (-6)-7 (-6)-6 (-6)-5 (-2)-4 (-2)-3 (-2)-2 (-2)-1 (2)0 (2)1 (2)2 (2)3 (6)4 (6)5 (6)6 (6)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = 6 Zs =   (-6)-8 (-6)-7 (-6)-6 (-6)-5 (-2)-4 (-2)-3 (-2)-2 (-2)-1 (2)0 (2)1 (2)2 (2)3 (6)4 (6)5 (6)6 (6)7</t>
+  </si>
+  <si>
+    <t>10:40:15 [INFO] ChunkX = 7 Zs =   (-6)-8 (-6)-7 (-6)-6 (-6)-5 (-2)-4 (-2)-3 (-2)-2 (-2)-1 (2)0 (2)1 (2)2 (2)3 (6)4 (6)5 (6)6 (6)7</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = -8 Zs =  -8/-8(N-W-) -8/-7(N---) -8/-6(N---) -8/-5(N--E) -4/-4(N-W-) -4/-3(N---) -4/-2(N---) -4/-1(N--E) 0/0(N-W-) 0/1(N---) 0/2(N---) 0/3(N--E) 4/4(N-W-) 4/5(N---) 4/6(N---) 4/7(N--E)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = -8 Zs =  -8/-8(--W-) -8/-7(----) -8/-6(----) -8/-5(---E) -4/-4(--W-) -4/-3(----) -4/-2(----) -4/-1(---E) 0/0(--W-) 0/1(----) 0/2(----) 0/3(---E) 4/4(--W-) 4/5(----) 4/6(----) 4/7(---E)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = -8 Zs =  -8/-8(-SW-) -8/-7(-S--) -8/-6(-S--) -8/-5(-S-E) -4/-4(-SW-) -4/-3(-S--) -4/-2(-S--) -4/-1(-S-E) 0/0(-SW-) 0/1(-S--) 0/2(-S--) 0/3(-S-E) 4/4(-SW-) 4/5(-S--) 4/6(-S--) 4/7(-S-E)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = -4 Zs =  -6/-8(N---) -6/-7(N---) -6/-6(N-W-) -6/-5(N---) -2/-4(N---) -2/-3(N---) -2/-2(N-W-) -2/-1(N---) 2/0(N---) 2/1(N---) 2/2(N-W-) 2/3(N---) 6/4(N---) 6/5(N---) 6/6(N-W-) 6/7(N---)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = -4 Zs =  -6/-8(----) -6/-7(----) -6/-6(--W-) -6/-5(----) -2/-4(----) -2/-3(----) -2/-2(--W-) -2/-1(----) 2/0(----) 2/1(----) 2/2(--W-) 2/3(----) 6/4(----) 6/5(----) 6/6(--W-) 6/7(----)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = -4 Zs =  -6/-8(-S--) -6/-7(-S--) -6/-6(-SW-) -6/-5(-S--) -2/-4(-S--) -2/-3(-S--) -2/-2(-SW-) -2/-1(-S--) 2/0(-S--) 2/1(-S--) 2/2(-SW-) 2/3(-S--) 6/4(-S--) 6/5(-S--) 6/6(-SW-) 6/7(-S--)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = 0 Zs =  -8/-8(N-W-) -8/-7(N---) -8/-6(N---) -8/-5(N--E) -4/-4(N-W-) -4/-3(N---) -4/-2(N---) -4/-1(N--E) 0/0(N-W-) 0/1(N---) 0/2(N---) 0/3(N--E) 4/4(N-W-) 4/5(N---) 4/6(N---) 4/7(N--E)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = 0 Zs =  -8/-8(--W-) -8/-7(----) -8/-6(----) -8/-5(---E) -4/-4(--W-) -4/-3(----) -4/-2(----) -4/-1(---E) 0/0(--W-) 0/1(----) 0/2(----) 0/3(---E) 4/4(--W-) 4/5(----) 4/6(----) 4/7(---E)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = 0 Zs =  -8/-8(-SW-) -8/-7(-S--) -8/-6(-S--) -8/-5(-S-E) -4/-4(-SW-) -4/-3(-S--) -4/-2(-S--) -4/-1(-S-E) 0/0(-SW-) 0/1(-S--) 0/2(-S--) 0/3(-S-E) 4/4(-SW-) 4/5(-S--) 4/6(-S--) 4/7(-S-E)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = 4 Zs =  -6/-8(N---) -6/-7(N---) -6/-6(N-W-) -6/-5(N---) -2/-4(N---) -2/-3(N---) -2/-2(N-W-) -2/-1(N---) 2/0(N---) 2/1(N---) 2/2(N-W-) 2/3(N---) 6/4(N---) 6/5(N---) 6/6(N-W-) 6/7(N---)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = 4 Zs =  -6/-8(----) -6/-7(----) -6/-6(--W-) -6/-5(----) -2/-4(----) -2/-3(----) -2/-2(--W-) -2/-1(----) 2/0(----) 2/1(----) 2/2(--W-) 2/3(----) 6/4(----) 6/5(----) 6/6(--W-) 6/7(----)</t>
+  </si>
+  <si>
+    <t>11:00:03 [INFO] WellX = 4 Zs =  -6/-8(-S--) -6/-7(-S--) -6/-6(-SW-) -6/-5(-S--) -2/-4(-S--) -2/-3(-S--) -2/-2(-SW-) -2/-1(-S--) 2/0(-S--) 2/1(-S--) 2/2(-SW-) 2/3(-S--) 6/4(-S--) 6/5(-S--) 6/6(-SW-) 6/7(-S--)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -592,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
@@ -781,6 +898,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" textRotation="180" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1227,11 +1378,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="186800384"/>
-        <c:axId val="186830848"/>
+        <c:axId val="266967296"/>
+        <c:axId val="266969088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="186800384"/>
+        <c:axId val="266967296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1240,7 +1391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186830848"/>
+        <c:crossAx val="266969088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1248,7 +1399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186830848"/>
+        <c:axId val="266969088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,7 +1410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186800384"/>
+        <c:crossAx val="266967296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2170,7 +2321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -4500,6 +4651,1233 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>-WellWidth2*2</f>
+        <v>-8</v>
+      </c>
+      <c r="B5">
+        <v>-8</v>
+      </c>
+      <c r="C5">
+        <v>-6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>+A5+1</f>
+        <v>-7</v>
+      </c>
+      <c r="B6">
+        <v>-8</v>
+      </c>
+      <c r="C6">
+        <v>-6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" ref="A7:A24" si="0">+A6+1</f>
+        <v>-6</v>
+      </c>
+      <c r="B7">
+        <v>-8</v>
+      </c>
+      <c r="C7">
+        <v>-6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="B8">
+        <v>-8</v>
+      </c>
+      <c r="C8">
+        <v>-6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="B9">
+        <v>-4</v>
+      </c>
+      <c r="C9">
+        <v>-2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="B10">
+        <v>-4</v>
+      </c>
+      <c r="C10">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="B11">
+        <v>-4</v>
+      </c>
+      <c r="C11">
+        <v>-2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="B12">
+        <v>-4</v>
+      </c>
+      <c r="C12">
+        <v>-2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E21" s="131" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E22" s="131" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E23" s="131" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E24" s="131" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E25" s="131" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E26" s="131" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E27" s="131" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E28" s="131" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E29" s="131" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E30" s="131" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E31" s="131" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E32" s="131" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="131" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="131" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="131" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="131" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:W21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="19" width="2.77734375" style="135"/>
+    <col min="20" max="21" width="2.77734375" style="135" customWidth="1"/>
+    <col min="22" max="16384" width="2.77734375" style="135"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B2" s="132"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="133"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="132"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="132"/>
+      <c r="S2" s="133"/>
+      <c r="T2" s="133"/>
+      <c r="U2" s="134"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B3" s="136"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="137"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="136"/>
+      <c r="O3" s="137"/>
+      <c r="P3" s="137"/>
+      <c r="Q3" s="138"/>
+      <c r="R3" s="136"/>
+      <c r="S3" s="137"/>
+      <c r="T3" s="137"/>
+      <c r="U3" s="138"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B4" s="136"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="137"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="137"/>
+      <c r="M4" s="138"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="137"/>
+      <c r="P4" s="137"/>
+      <c r="Q4" s="138"/>
+      <c r="R4" s="136"/>
+      <c r="S4" s="137"/>
+      <c r="T4" s="137"/>
+      <c r="U4" s="138"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B5" s="139"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="140"/>
+      <c r="H5" s="140"/>
+      <c r="I5" s="141"/>
+      <c r="J5" s="139"/>
+      <c r="K5" s="140"/>
+      <c r="L5" s="140"/>
+      <c r="M5" s="141"/>
+      <c r="N5" s="139"/>
+      <c r="O5" s="140"/>
+      <c r="P5" s="140"/>
+      <c r="Q5" s="141"/>
+      <c r="R5" s="139"/>
+      <c r="S5" s="140"/>
+      <c r="T5" s="140"/>
+      <c r="U5" s="141"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="D6" s="132"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
+      <c r="K6" s="134"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="133"/>
+      <c r="N6" s="133"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="133"/>
+      <c r="R6" s="133"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="132"/>
+      <c r="U6" s="133"/>
+      <c r="V6" s="133"/>
+      <c r="W6" s="134"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="D7" s="136">
+        <f t="shared" ref="D7" si="0">D9-D8</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="137">
+        <f t="shared" ref="E7" si="1">E9-E8</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="137">
+        <f t="shared" ref="F7" si="2">F9-F8</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="138">
+        <f t="shared" ref="G7" si="3">G9-G8</f>
+        <v>3</v>
+      </c>
+      <c r="H7" s="136">
+        <f t="shared" ref="H7" si="4">H9-H8</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="137">
+        <f t="shared" ref="I7" si="5">I9-I8</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="137">
+        <f t="shared" ref="J7" si="6">J9-J8</f>
+        <v>2</v>
+      </c>
+      <c r="K7" s="138">
+        <f t="shared" ref="K7" si="7">K9-K8</f>
+        <v>3</v>
+      </c>
+      <c r="L7" s="136">
+        <f t="shared" ref="L7" si="8">L9-L8</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="137">
+        <f t="shared" ref="M7" si="9">M9-M8</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="137">
+        <f t="shared" ref="N7" si="10">N9-N8</f>
+        <v>2</v>
+      </c>
+      <c r="O7" s="138">
+        <f t="shared" ref="O7" si="11">O9-O8</f>
+        <v>3</v>
+      </c>
+      <c r="P7" s="136">
+        <f t="shared" ref="P7" si="12">P9-P8</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="137">
+        <f t="shared" ref="Q7" si="13">Q9-Q8</f>
+        <v>1</v>
+      </c>
+      <c r="R7" s="137">
+        <f t="shared" ref="R7" si="14">R9-R8</f>
+        <v>2</v>
+      </c>
+      <c r="S7" s="138">
+        <f t="shared" ref="S7" si="15">S9-S8</f>
+        <v>3</v>
+      </c>
+      <c r="T7" s="136">
+        <f t="shared" ref="T7" si="16">T9-T8</f>
+        <v>0</v>
+      </c>
+      <c r="U7" s="137">
+        <f t="shared" ref="U7" si="17">U9-U8</f>
+        <v>1</v>
+      </c>
+      <c r="V7" s="137">
+        <f t="shared" ref="V7" si="18">V9-V8</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="138">
+        <f t="shared" ref="W7" si="19">W9-W8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="D8" s="136">
+        <v>-6</v>
+      </c>
+      <c r="E8" s="137">
+        <v>-6</v>
+      </c>
+      <c r="F8" s="137">
+        <v>-6</v>
+      </c>
+      <c r="G8" s="138">
+        <v>-6</v>
+      </c>
+      <c r="H8" s="136">
+        <v>-2</v>
+      </c>
+      <c r="I8" s="137">
+        <v>-2</v>
+      </c>
+      <c r="J8" s="137">
+        <v>-2</v>
+      </c>
+      <c r="K8" s="138">
+        <v>-2</v>
+      </c>
+      <c r="L8" s="136">
+        <v>2</v>
+      </c>
+      <c r="M8" s="142">
+        <v>2</v>
+      </c>
+      <c r="N8" s="142">
+        <v>2</v>
+      </c>
+      <c r="O8" s="138">
+        <v>2</v>
+      </c>
+      <c r="P8" s="136">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="142">
+        <v>6</v>
+      </c>
+      <c r="R8" s="142">
+        <v>6</v>
+      </c>
+      <c r="S8" s="138">
+        <v>6</v>
+      </c>
+      <c r="T8" s="136">
+        <v>10</v>
+      </c>
+      <c r="U8" s="142">
+        <v>10</v>
+      </c>
+      <c r="V8" s="137"/>
+      <c r="W8" s="138"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B9" s="135">
+        <f t="shared" ref="B9:H9" si="20">C9-1</f>
+        <v>-8</v>
+      </c>
+      <c r="C9" s="135">
+        <f t="shared" si="20"/>
+        <v>-7</v>
+      </c>
+      <c r="D9" s="139">
+        <f t="shared" si="20"/>
+        <v>-6</v>
+      </c>
+      <c r="E9" s="140">
+        <f t="shared" si="20"/>
+        <v>-5</v>
+      </c>
+      <c r="F9" s="140">
+        <f t="shared" si="20"/>
+        <v>-4</v>
+      </c>
+      <c r="G9" s="141">
+        <f t="shared" si="20"/>
+        <v>-3</v>
+      </c>
+      <c r="H9" s="139">
+        <f t="shared" si="20"/>
+        <v>-2</v>
+      </c>
+      <c r="I9" s="140">
+        <f>J9-1</f>
+        <v>-1</v>
+      </c>
+      <c r="J9" s="140">
+        <v>0</v>
+      </c>
+      <c r="K9" s="141">
+        <f>J9+1</f>
+        <v>1</v>
+      </c>
+      <c r="L9" s="139">
+        <f t="shared" ref="L9:U9" si="21">K9+1</f>
+        <v>2</v>
+      </c>
+      <c r="M9" s="140">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="N9" s="140">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="O9" s="141">
+        <f t="shared" si="21"/>
+        <v>5</v>
+      </c>
+      <c r="P9" s="139">
+        <f t="shared" si="21"/>
+        <v>6</v>
+      </c>
+      <c r="Q9" s="140">
+        <f t="shared" si="21"/>
+        <v>7</v>
+      </c>
+      <c r="R9" s="140">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="S9" s="141">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="T9" s="139">
+        <f t="shared" si="21"/>
+        <v>10</v>
+      </c>
+      <c r="U9" s="140">
+        <f t="shared" si="21"/>
+        <v>11</v>
+      </c>
+      <c r="V9" s="140"/>
+      <c r="W9" s="141"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B10" s="132"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="134"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="132"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="133"/>
+      <c r="M10" s="134"/>
+      <c r="N10" s="132"/>
+      <c r="O10" s="133"/>
+      <c r="P10" s="133"/>
+      <c r="Q10" s="134"/>
+      <c r="R10" s="132"/>
+      <c r="S10" s="133"/>
+      <c r="T10" s="133"/>
+      <c r="U10" s="134"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B11" s="136">
+        <f t="shared" ref="B11" si="22">B13-B12</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="137">
+        <f t="shared" ref="C11" si="23">C13-C12</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="137">
+        <f t="shared" ref="D11" si="24">D13-D12</f>
+        <v>2</v>
+      </c>
+      <c r="E11" s="138">
+        <f t="shared" ref="E11:F11" si="25">E13-E12</f>
+        <v>3</v>
+      </c>
+      <c r="F11" s="136">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="137">
+        <f t="shared" ref="G11" si="26">G13-G12</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="137">
+        <f t="shared" ref="H11" si="27">H13-H12</f>
+        <v>2</v>
+      </c>
+      <c r="I11" s="138">
+        <f t="shared" ref="I11" si="28">I13-I12</f>
+        <v>3</v>
+      </c>
+      <c r="J11" s="136">
+        <f>J13-J12</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="137">
+        <f t="shared" ref="K11:N11" si="29">K13-K12</f>
+        <v>1</v>
+      </c>
+      <c r="L11" s="137">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="M11" s="138">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="N11" s="136">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="137">
+        <f t="shared" ref="O11" si="30">O13-O12</f>
+        <v>1</v>
+      </c>
+      <c r="P11" s="137">
+        <f t="shared" ref="P11" si="31">P13-P12</f>
+        <v>2</v>
+      </c>
+      <c r="Q11" s="138">
+        <f t="shared" ref="Q11:R11" si="32">Q13-Q12</f>
+        <v>3</v>
+      </c>
+      <c r="R11" s="136">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="S11" s="137">
+        <f t="shared" ref="S11" si="33">S13-S12</f>
+        <v>1</v>
+      </c>
+      <c r="T11" s="137">
+        <f t="shared" ref="T11" si="34">T13-T12</f>
+        <v>2</v>
+      </c>
+      <c r="U11" s="138">
+        <f t="shared" ref="U11" si="35">U13-U12</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B12" s="136">
+        <v>-8</v>
+      </c>
+      <c r="C12" s="137">
+        <v>-8</v>
+      </c>
+      <c r="D12" s="137">
+        <v>-8</v>
+      </c>
+      <c r="E12" s="138">
+        <v>-8</v>
+      </c>
+      <c r="F12" s="136">
+        <v>-4</v>
+      </c>
+      <c r="G12" s="137">
+        <v>-4</v>
+      </c>
+      <c r="H12" s="137">
+        <v>-4</v>
+      </c>
+      <c r="I12" s="138">
+        <v>-4</v>
+      </c>
+      <c r="J12" s="136">
+        <v>0</v>
+      </c>
+      <c r="K12" s="137">
+        <v>0</v>
+      </c>
+      <c r="L12" s="137">
+        <v>0</v>
+      </c>
+      <c r="M12" s="138">
+        <v>0</v>
+      </c>
+      <c r="N12" s="136">
+        <v>4</v>
+      </c>
+      <c r="O12" s="142">
+        <v>4</v>
+      </c>
+      <c r="P12" s="142">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="138">
+        <v>4</v>
+      </c>
+      <c r="R12" s="136">
+        <v>8</v>
+      </c>
+      <c r="S12" s="142">
+        <v>8</v>
+      </c>
+      <c r="T12" s="142">
+        <v>8</v>
+      </c>
+      <c r="U12" s="138">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B13" s="139">
+        <f t="shared" ref="B13:H13" si="36">C13-1</f>
+        <v>-8</v>
+      </c>
+      <c r="C13" s="140">
+        <f t="shared" si="36"/>
+        <v>-7</v>
+      </c>
+      <c r="D13" s="140">
+        <f t="shared" si="36"/>
+        <v>-6</v>
+      </c>
+      <c r="E13" s="141">
+        <f t="shared" si="36"/>
+        <v>-5</v>
+      </c>
+      <c r="F13" s="139">
+        <f t="shared" si="36"/>
+        <v>-4</v>
+      </c>
+      <c r="G13" s="140">
+        <f t="shared" si="36"/>
+        <v>-3</v>
+      </c>
+      <c r="H13" s="140">
+        <f t="shared" si="36"/>
+        <v>-2</v>
+      </c>
+      <c r="I13" s="141">
+        <f>J13-1</f>
+        <v>-1</v>
+      </c>
+      <c r="J13" s="139">
+        <v>0</v>
+      </c>
+      <c r="K13" s="140">
+        <f>J13+1</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="140">
+        <f t="shared" ref="L13:U13" si="37">K13+1</f>
+        <v>2</v>
+      </c>
+      <c r="M13" s="141">
+        <f t="shared" si="37"/>
+        <v>3</v>
+      </c>
+      <c r="N13" s="139">
+        <f t="shared" si="37"/>
+        <v>4</v>
+      </c>
+      <c r="O13" s="140">
+        <f t="shared" si="37"/>
+        <v>5</v>
+      </c>
+      <c r="P13" s="140">
+        <f t="shared" si="37"/>
+        <v>6</v>
+      </c>
+      <c r="Q13" s="141">
+        <f t="shared" si="37"/>
+        <v>7</v>
+      </c>
+      <c r="R13" s="139">
+        <f t="shared" si="37"/>
+        <v>8</v>
+      </c>
+      <c r="S13" s="140">
+        <f t="shared" si="37"/>
+        <v>9</v>
+      </c>
+      <c r="T13" s="140">
+        <f t="shared" si="37"/>
+        <v>10</v>
+      </c>
+      <c r="U13" s="141">
+        <f t="shared" si="37"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="D14" s="132"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="134"/>
+      <c r="H14" s="132"/>
+      <c r="I14" s="133"/>
+      <c r="J14" s="133"/>
+      <c r="K14" s="134"/>
+      <c r="L14" s="132"/>
+      <c r="M14" s="133"/>
+      <c r="N14" s="133"/>
+      <c r="O14" s="134"/>
+      <c r="P14" s="132"/>
+      <c r="Q14" s="133"/>
+      <c r="R14" s="133"/>
+      <c r="S14" s="134"/>
+      <c r="T14" s="132"/>
+      <c r="U14" s="133"/>
+      <c r="V14" s="133"/>
+      <c r="W14" s="134"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="D15" s="136"/>
+      <c r="E15" s="137"/>
+      <c r="F15" s="137"/>
+      <c r="G15" s="138"/>
+      <c r="H15" s="136"/>
+      <c r="I15" s="137"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="138"/>
+      <c r="L15" s="136"/>
+      <c r="M15" s="137"/>
+      <c r="N15" s="137"/>
+      <c r="O15" s="138"/>
+      <c r="P15" s="136"/>
+      <c r="Q15" s="137"/>
+      <c r="R15" s="137"/>
+      <c r="S15" s="138"/>
+      <c r="T15" s="136"/>
+      <c r="U15" s="137"/>
+      <c r="V15" s="137"/>
+      <c r="W15" s="138"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="D16" s="136"/>
+      <c r="E16" s="137"/>
+      <c r="F16" s="137"/>
+      <c r="G16" s="138"/>
+      <c r="H16" s="136"/>
+      <c r="I16" s="137"/>
+      <c r="J16" s="137"/>
+      <c r="K16" s="138"/>
+      <c r="L16" s="136"/>
+      <c r="M16" s="137"/>
+      <c r="N16" s="137"/>
+      <c r="O16" s="138"/>
+      <c r="P16" s="136"/>
+      <c r="Q16" s="137"/>
+      <c r="R16" s="137"/>
+      <c r="S16" s="138"/>
+      <c r="T16" s="136"/>
+      <c r="U16" s="137"/>
+      <c r="V16" s="137"/>
+      <c r="W16" s="138"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B17" s="135">
+        <f t="shared" ref="B17:H17" si="38">C17-1</f>
+        <v>-8</v>
+      </c>
+      <c r="C17" s="135">
+        <f t="shared" si="38"/>
+        <v>-7</v>
+      </c>
+      <c r="D17" s="139">
+        <f t="shared" si="38"/>
+        <v>-6</v>
+      </c>
+      <c r="E17" s="140">
+        <f t="shared" si="38"/>
+        <v>-5</v>
+      </c>
+      <c r="F17" s="140">
+        <f t="shared" si="38"/>
+        <v>-4</v>
+      </c>
+      <c r="G17" s="141">
+        <f t="shared" si="38"/>
+        <v>-3</v>
+      </c>
+      <c r="H17" s="139">
+        <f t="shared" si="38"/>
+        <v>-2</v>
+      </c>
+      <c r="I17" s="140">
+        <f>J17-1</f>
+        <v>-1</v>
+      </c>
+      <c r="J17" s="140">
+        <v>0</v>
+      </c>
+      <c r="K17" s="141">
+        <f>J17+1</f>
+        <v>1</v>
+      </c>
+      <c r="L17" s="139">
+        <f t="shared" ref="L17:U17" si="39">K17+1</f>
+        <v>2</v>
+      </c>
+      <c r="M17" s="140">
+        <f t="shared" si="39"/>
+        <v>3</v>
+      </c>
+      <c r="N17" s="140">
+        <f t="shared" si="39"/>
+        <v>4</v>
+      </c>
+      <c r="O17" s="141">
+        <f t="shared" si="39"/>
+        <v>5</v>
+      </c>
+      <c r="P17" s="139">
+        <f t="shared" si="39"/>
+        <v>6</v>
+      </c>
+      <c r="Q17" s="140">
+        <f t="shared" si="39"/>
+        <v>7</v>
+      </c>
+      <c r="R17" s="140">
+        <f t="shared" si="39"/>
+        <v>8</v>
+      </c>
+      <c r="S17" s="141">
+        <f t="shared" si="39"/>
+        <v>9</v>
+      </c>
+      <c r="T17" s="139">
+        <f t="shared" si="39"/>
+        <v>10</v>
+      </c>
+      <c r="U17" s="140">
+        <f t="shared" si="39"/>
+        <v>11</v>
+      </c>
+      <c r="V17" s="140"/>
+      <c r="W17" s="141"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B18" s="132"/>
+      <c r="C18" s="133"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="134"/>
+      <c r="F18" s="132"/>
+      <c r="G18" s="133"/>
+      <c r="H18" s="133"/>
+      <c r="I18" s="134"/>
+      <c r="J18" s="132"/>
+      <c r="K18" s="133"/>
+      <c r="L18" s="133"/>
+      <c r="M18" s="134"/>
+      <c r="N18" s="132"/>
+      <c r="O18" s="133"/>
+      <c r="P18" s="133"/>
+      <c r="Q18" s="134"/>
+      <c r="R18" s="132"/>
+      <c r="S18" s="133"/>
+      <c r="T18" s="133"/>
+      <c r="U18" s="134"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B19" s="136"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="137"/>
+      <c r="E19" s="138"/>
+      <c r="F19" s="136"/>
+      <c r="G19" s="137"/>
+      <c r="H19" s="137"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="136"/>
+      <c r="K19" s="137"/>
+      <c r="L19" s="137"/>
+      <c r="M19" s="138"/>
+      <c r="N19" s="136"/>
+      <c r="O19" s="137"/>
+      <c r="P19" s="137"/>
+      <c r="Q19" s="138"/>
+      <c r="R19" s="136"/>
+      <c r="S19" s="137"/>
+      <c r="T19" s="137"/>
+      <c r="U19" s="138"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B20" s="136"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="138"/>
+      <c r="F20" s="136"/>
+      <c r="G20" s="137"/>
+      <c r="H20" s="137"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="136"/>
+      <c r="K20" s="137"/>
+      <c r="L20" s="137"/>
+      <c r="M20" s="138"/>
+      <c r="N20" s="136"/>
+      <c r="O20" s="137"/>
+      <c r="P20" s="137"/>
+      <c r="Q20" s="138"/>
+      <c r="R20" s="136"/>
+      <c r="S20" s="137"/>
+      <c r="T20" s="137"/>
+      <c r="U20" s="138"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B21" s="139"/>
+      <c r="C21" s="140"/>
+      <c r="D21" s="140"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="140"/>
+      <c r="H21" s="140"/>
+      <c r="I21" s="141"/>
+      <c r="J21" s="139"/>
+      <c r="K21" s="140"/>
+      <c r="L21" s="140"/>
+      <c r="M21" s="141"/>
+      <c r="N21" s="139"/>
+      <c r="O21" s="140"/>
+      <c r="P21" s="140"/>
+      <c r="Q21" s="141"/>
+      <c r="R21" s="139"/>
+      <c r="S21" s="140"/>
+      <c r="T21" s="140"/>
+      <c r="U21" s="141"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Now with YML config!
</commit_message>
<xml_diff>
--- a/notes/WellThoughts.xlsx
+++ b/notes/WellThoughts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="16260" windowHeight="9000" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="16260" windowHeight="8940" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Oddz" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,19 @@
     <sheet name="VolcanoShape" sheetId="10" r:id="rId10"/>
     <sheet name="HexCalc2" sheetId="11" r:id="rId11"/>
     <sheet name="Sheet2" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="HalfPi">VolcanoShape!$F$2</definedName>
+    <definedName name="incer">Sheet1!$A$3</definedName>
+    <definedName name="range">Sheet1!$A$2</definedName>
     <definedName name="Steps">VolcanoShape!$G$1</definedName>
     <definedName name="TwoPi">VolcanoShape!$F$1</definedName>
     <definedName name="WellWidth">'Hex step'!$A$1</definedName>
     <definedName name="WellWidth2">HexCalc2!$B$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -893,12 +897,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" textRotation="180" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
@@ -932,6 +930,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" textRotation="180" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1378,11 +1382,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="266967296"/>
-        <c:axId val="266969088"/>
+        <c:axId val="222466048"/>
+        <c:axId val="222467584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="266967296"/>
+        <c:axId val="222466048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,7 +1395,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266969088"/>
+        <c:crossAx val="222467584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1399,7 +1403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="266969088"/>
+        <c:axId val="222467584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1410,14 +1414,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266967296"/>
+        <c:crossAx val="222466048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1772,10 +1775,10 @@
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="129" t="s">
+      <c r="P1" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="129"/>
+      <c r="Q1" s="141"/>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -1855,7 +1858,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="10"/>
-      <c r="L5" s="130" t="s">
+      <c r="L5" s="142" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="1">
@@ -1904,7 +1907,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="10"/>
-      <c r="L6" s="130"/>
+      <c r="L6" s="142"/>
       <c r="O6" s="6"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="9"/>
@@ -4947,7 +4950,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E21" s="131" t="s">
+      <c r="E21" s="129" t="s">
         <v>54</v>
       </c>
     </row>
@@ -4956,7 +4959,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="129" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4965,7 +4968,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E23" s="131" t="s">
+      <c r="E23" s="129" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4974,67 +4977,67 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E24" s="131" t="s">
+      <c r="E24" s="129" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E25" s="131" t="s">
+      <c r="E25" s="129" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E26" s="131" t="s">
+      <c r="E26" s="129" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E27" s="131" t="s">
+      <c r="E27" s="129" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E28" s="131" t="s">
+      <c r="E28" s="129" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E29" s="131" t="s">
+      <c r="E29" s="129" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E30" s="131" t="s">
+      <c r="E30" s="129" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E31" s="131" t="s">
+      <c r="E31" s="129" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E32" s="131" t="s">
+      <c r="E32" s="129" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E33" s="131" t="s">
+      <c r="E33" s="129" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E34" s="131" t="s">
+      <c r="E34" s="129" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E35" s="131" t="s">
+      <c r="E35" s="129" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E36" s="131" t="s">
+      <c r="E36" s="129" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5048,833 +5051,2059 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AH19" sqref="AH19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="19" width="2.77734375" style="135"/>
-    <col min="20" max="21" width="2.77734375" style="135" customWidth="1"/>
-    <col min="22" max="16384" width="2.77734375" style="135"/>
+    <col min="1" max="19" width="2.77734375" style="133"/>
+    <col min="20" max="21" width="2.77734375" style="133" customWidth="1"/>
+    <col min="22" max="16384" width="2.77734375" style="133"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="132"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="132"/>
-      <c r="O2" s="133"/>
-      <c r="P2" s="133"/>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="132"/>
-      <c r="S2" s="133"/>
-      <c r="T2" s="133"/>
-      <c r="U2" s="134"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="132"/>
+      <c r="N2" s="130"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="132"/>
+      <c r="R2" s="130"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="131"/>
+      <c r="U2" s="132"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="136"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="138"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="137"/>
-      <c r="L3" s="137"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="136"/>
-      <c r="O3" s="137"/>
-      <c r="P3" s="137"/>
-      <c r="Q3" s="138"/>
-      <c r="R3" s="136"/>
-      <c r="S3" s="137"/>
-      <c r="T3" s="137"/>
-      <c r="U3" s="138"/>
+      <c r="B3" s="134"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="134"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="136"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="135"/>
+      <c r="P3" s="135"/>
+      <c r="Q3" s="136"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="135"/>
+      <c r="T3" s="135"/>
+      <c r="U3" s="136"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="136"/>
-      <c r="C4" s="137"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="137"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="137"/>
-      <c r="L4" s="137"/>
-      <c r="M4" s="138"/>
-      <c r="N4" s="136"/>
-      <c r="O4" s="137"/>
-      <c r="P4" s="137"/>
-      <c r="Q4" s="138"/>
-      <c r="R4" s="136"/>
-      <c r="S4" s="137"/>
-      <c r="T4" s="137"/>
-      <c r="U4" s="138"/>
+      <c r="B4" s="134"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="135"/>
+      <c r="L4" s="135"/>
+      <c r="M4" s="136"/>
+      <c r="N4" s="134"/>
+      <c r="O4" s="135"/>
+      <c r="P4" s="135"/>
+      <c r="Q4" s="136"/>
+      <c r="R4" s="134"/>
+      <c r="S4" s="135"/>
+      <c r="T4" s="135"/>
+      <c r="U4" s="136"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="139"/>
-      <c r="C5" s="140"/>
-      <c r="D5" s="140"/>
-      <c r="E5" s="141"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="140"/>
-      <c r="H5" s="140"/>
-      <c r="I5" s="141"/>
-      <c r="J5" s="139"/>
-      <c r="K5" s="140"/>
-      <c r="L5" s="140"/>
-      <c r="M5" s="141"/>
-      <c r="N5" s="139"/>
-      <c r="O5" s="140"/>
-      <c r="P5" s="140"/>
-      <c r="Q5" s="141"/>
-      <c r="R5" s="139"/>
-      <c r="S5" s="140"/>
-      <c r="T5" s="140"/>
-      <c r="U5" s="141"/>
+      <c r="B5" s="137"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="137"/>
+      <c r="G5" s="138"/>
+      <c r="H5" s="138"/>
+      <c r="I5" s="139"/>
+      <c r="J5" s="137"/>
+      <c r="K5" s="138"/>
+      <c r="L5" s="138"/>
+      <c r="M5" s="139"/>
+      <c r="N5" s="137"/>
+      <c r="O5" s="138"/>
+      <c r="P5" s="138"/>
+      <c r="Q5" s="139"/>
+      <c r="R5" s="137"/>
+      <c r="S5" s="138"/>
+      <c r="T5" s="138"/>
+      <c r="U5" s="139"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D6" s="132"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="133"/>
-      <c r="J6" s="133"/>
-      <c r="K6" s="134"/>
-      <c r="L6" s="132"/>
-      <c r="M6" s="133"/>
-      <c r="N6" s="133"/>
-      <c r="O6" s="134"/>
-      <c r="P6" s="132"/>
-      <c r="Q6" s="133"/>
-      <c r="R6" s="133"/>
-      <c r="S6" s="134"/>
-      <c r="T6" s="132"/>
-      <c r="U6" s="133"/>
-      <c r="V6" s="133"/>
-      <c r="W6" s="134"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="130"/>
+      <c r="M6" s="131"/>
+      <c r="N6" s="131"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="130"/>
+      <c r="Q6" s="131"/>
+      <c r="R6" s="131"/>
+      <c r="S6" s="132"/>
+      <c r="T6" s="130"/>
+      <c r="U6" s="131"/>
+      <c r="V6" s="131"/>
+      <c r="W6" s="132"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D7" s="136">
-        <f t="shared" ref="D7" si="0">D9-D8</f>
+      <c r="D7" s="134">
+        <f t="shared" ref="D7:W7" si="0">D9-D8</f>
         <v>0</v>
       </c>
-      <c r="E7" s="137">
-        <f t="shared" ref="E7" si="1">E9-E8</f>
+      <c r="E7" s="135">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F7" s="137">
-        <f t="shared" ref="F7" si="2">F9-F8</f>
+      <c r="F7" s="135">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G7" s="138">
-        <f t="shared" ref="G7" si="3">G9-G8</f>
+      <c r="G7" s="136">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H7" s="136">
-        <f t="shared" ref="H7" si="4">H9-H8</f>
+      <c r="H7" s="134">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="137">
-        <f t="shared" ref="I7" si="5">I9-I8</f>
+      <c r="I7" s="135">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J7" s="137">
-        <f t="shared" ref="J7" si="6">J9-J8</f>
+      <c r="J7" s="135">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K7" s="138">
-        <f t="shared" ref="K7" si="7">K9-K8</f>
+      <c r="K7" s="136">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L7" s="136">
-        <f t="shared" ref="L7" si="8">L9-L8</f>
+      <c r="L7" s="134">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M7" s="137">
-        <f t="shared" ref="M7" si="9">M9-M8</f>
+      <c r="M7" s="135">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N7" s="137">
-        <f t="shared" ref="N7" si="10">N9-N8</f>
+      <c r="N7" s="135">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="O7" s="138">
-        <f t="shared" ref="O7" si="11">O9-O8</f>
+      <c r="O7" s="136">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P7" s="136">
-        <f t="shared" ref="P7" si="12">P9-P8</f>
+      <c r="P7" s="134">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="137">
-        <f t="shared" ref="Q7" si="13">Q9-Q8</f>
+      <c r="Q7" s="135">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="R7" s="137">
-        <f t="shared" ref="R7" si="14">R9-R8</f>
+      <c r="R7" s="135">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="S7" s="138">
-        <f t="shared" ref="S7" si="15">S9-S8</f>
+      <c r="S7" s="136">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="T7" s="136">
-        <f t="shared" ref="T7" si="16">T9-T8</f>
+      <c r="T7" s="134">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U7" s="137">
-        <f t="shared" ref="U7" si="17">U9-U8</f>
+      <c r="U7" s="135">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V7" s="137">
-        <f t="shared" ref="V7" si="18">V9-V8</f>
+      <c r="V7" s="135">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W7" s="138">
-        <f t="shared" ref="W7" si="19">W9-W8</f>
+      <c r="W7" s="136">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D8" s="136">
+      <c r="D8" s="134">
         <v>-6</v>
       </c>
-      <c r="E8" s="137">
+      <c r="E8" s="135">
         <v>-6</v>
       </c>
-      <c r="F8" s="137">
+      <c r="F8" s="135">
         <v>-6</v>
       </c>
-      <c r="G8" s="138">
+      <c r="G8" s="136">
         <v>-6</v>
       </c>
-      <c r="H8" s="136">
+      <c r="H8" s="134">
         <v>-2</v>
       </c>
-      <c r="I8" s="137">
+      <c r="I8" s="135">
         <v>-2</v>
       </c>
-      <c r="J8" s="137">
+      <c r="J8" s="135">
         <v>-2</v>
       </c>
-      <c r="K8" s="138">
+      <c r="K8" s="136">
         <v>-2</v>
       </c>
-      <c r="L8" s="136">
+      <c r="L8" s="134">
         <v>2</v>
       </c>
-      <c r="M8" s="142">
+      <c r="M8" s="140">
         <v>2</v>
       </c>
-      <c r="N8" s="142">
+      <c r="N8" s="140">
         <v>2</v>
       </c>
-      <c r="O8" s="138">
+      <c r="O8" s="136">
         <v>2</v>
       </c>
-      <c r="P8" s="136">
+      <c r="P8" s="134">
         <v>6</v>
       </c>
-      <c r="Q8" s="142">
+      <c r="Q8" s="140">
         <v>6</v>
       </c>
-      <c r="R8" s="142">
+      <c r="R8" s="140">
         <v>6</v>
       </c>
-      <c r="S8" s="138">
+      <c r="S8" s="136">
         <v>6</v>
       </c>
-      <c r="T8" s="136">
+      <c r="T8" s="134">
         <v>10</v>
       </c>
-      <c r="U8" s="142">
+      <c r="U8" s="140">
         <v>10</v>
       </c>
-      <c r="V8" s="137"/>
-      <c r="W8" s="138"/>
+      <c r="V8" s="135"/>
+      <c r="W8" s="136"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B9" s="135">
-        <f t="shared" ref="B9:H9" si="20">C9-1</f>
+      <c r="B9" s="133">
+        <f t="shared" ref="B9:H9" si="1">C9-1</f>
         <v>-8</v>
       </c>
-      <c r="C9" s="135">
-        <f t="shared" si="20"/>
+      <c r="C9" s="133">
+        <f t="shared" si="1"/>
         <v>-7</v>
       </c>
-      <c r="D9" s="139">
-        <f t="shared" si="20"/>
+      <c r="D9" s="137">
+        <f t="shared" si="1"/>
         <v>-6</v>
       </c>
-      <c r="E9" s="140">
-        <f t="shared" si="20"/>
+      <c r="E9" s="138">
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="F9" s="140">
-        <f t="shared" si="20"/>
+      <c r="F9" s="138">
+        <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="G9" s="141">
-        <f t="shared" si="20"/>
+      <c r="G9" s="139">
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
-      <c r="H9" s="139">
-        <f t="shared" si="20"/>
+      <c r="H9" s="137">
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="I9" s="140">
+      <c r="I9" s="138">
         <f>J9-1</f>
         <v>-1</v>
       </c>
-      <c r="J9" s="140">
+      <c r="J9" s="138">
         <v>0</v>
       </c>
-      <c r="K9" s="141">
+      <c r="K9" s="139">
         <f>J9+1</f>
         <v>1</v>
       </c>
-      <c r="L9" s="139">
-        <f t="shared" ref="L9:U9" si="21">K9+1</f>
+      <c r="L9" s="137">
+        <f t="shared" ref="L9:U9" si="2">K9+1</f>
         <v>2</v>
       </c>
-      <c r="M9" s="140">
-        <f t="shared" si="21"/>
+      <c r="M9" s="138">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="N9" s="140">
-        <f t="shared" si="21"/>
+      <c r="N9" s="138">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="O9" s="141">
-        <f t="shared" si="21"/>
+      <c r="O9" s="139">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="P9" s="139">
-        <f t="shared" si="21"/>
+      <c r="P9" s="137">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="Q9" s="140">
-        <f t="shared" si="21"/>
+      <c r="Q9" s="138">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="R9" s="140">
-        <f t="shared" si="21"/>
+      <c r="R9" s="138">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="S9" s="141">
-        <f t="shared" si="21"/>
+      <c r="S9" s="139">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="T9" s="139">
-        <f t="shared" si="21"/>
+      <c r="T9" s="137">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="U9" s="140">
-        <f t="shared" si="21"/>
+      <c r="U9" s="138">
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="V9" s="140"/>
-      <c r="W9" s="141"/>
+      <c r="V9" s="138"/>
+      <c r="W9" s="139"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B10" s="132"/>
-      <c r="C10" s="133"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="134"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="133"/>
-      <c r="H10" s="133"/>
-      <c r="I10" s="134"/>
-      <c r="J10" s="132"/>
-      <c r="K10" s="133"/>
-      <c r="L10" s="133"/>
-      <c r="M10" s="134"/>
-      <c r="N10" s="132"/>
-      <c r="O10" s="133"/>
-      <c r="P10" s="133"/>
-      <c r="Q10" s="134"/>
-      <c r="R10" s="132"/>
-      <c r="S10" s="133"/>
-      <c r="T10" s="133"/>
-      <c r="U10" s="134"/>
+      <c r="B10" s="130"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="131"/>
+      <c r="H10" s="131"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="131"/>
+      <c r="L10" s="131"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="130"/>
+      <c r="O10" s="131"/>
+      <c r="P10" s="131"/>
+      <c r="Q10" s="132"/>
+      <c r="R10" s="130"/>
+      <c r="S10" s="131"/>
+      <c r="T10" s="131"/>
+      <c r="U10" s="132"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B11" s="136">
-        <f t="shared" ref="B11" si="22">B13-B12</f>
+      <c r="B11" s="134">
+        <f t="shared" ref="B11:U11" si="3">B13-B12</f>
         <v>0</v>
       </c>
-      <c r="C11" s="137">
-        <f t="shared" ref="C11" si="23">C13-C12</f>
+      <c r="C11" s="135">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="D11" s="137">
-        <f t="shared" ref="D11" si="24">D13-D12</f>
+      <c r="D11" s="135">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="E11" s="138">
-        <f t="shared" ref="E11:F11" si="25">E13-E12</f>
+      <c r="E11" s="136">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="F11" s="136">
-        <f t="shared" si="25"/>
+      <c r="F11" s="134">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G11" s="137">
-        <f t="shared" ref="G11" si="26">G13-G12</f>
+      <c r="G11" s="135">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="H11" s="137">
-        <f t="shared" ref="H11" si="27">H13-H12</f>
+      <c r="H11" s="135">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="I11" s="138">
-        <f t="shared" ref="I11" si="28">I13-I12</f>
+      <c r="I11" s="136">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="J11" s="136">
-        <f>J13-J12</f>
+      <c r="J11" s="134">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K11" s="137">
-        <f t="shared" ref="K11:N11" si="29">K13-K12</f>
+      <c r="K11" s="135">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L11" s="137">
-        <f t="shared" si="29"/>
+      <c r="L11" s="135">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M11" s="138">
-        <f t="shared" si="29"/>
+      <c r="M11" s="136">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="N11" s="136">
-        <f t="shared" si="29"/>
+      <c r="N11" s="134">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O11" s="137">
-        <f t="shared" ref="O11" si="30">O13-O12</f>
+      <c r="O11" s="135">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P11" s="137">
-        <f t="shared" ref="P11" si="31">P13-P12</f>
+      <c r="P11" s="135">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="Q11" s="138">
-        <f t="shared" ref="Q11:R11" si="32">Q13-Q12</f>
+      <c r="Q11" s="136">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="R11" s="136">
-        <f t="shared" si="32"/>
+      <c r="R11" s="134">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S11" s="137">
-        <f t="shared" ref="S11" si="33">S13-S12</f>
+      <c r="S11" s="135">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="T11" s="137">
-        <f t="shared" ref="T11" si="34">T13-T12</f>
+      <c r="T11" s="135">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="U11" s="138">
-        <f t="shared" ref="U11" si="35">U13-U12</f>
+      <c r="U11" s="136">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B12" s="136">
+      <c r="B12" s="134">
         <v>-8</v>
       </c>
-      <c r="C12" s="137">
+      <c r="C12" s="135">
         <v>-8</v>
       </c>
-      <c r="D12" s="137">
+      <c r="D12" s="135">
         <v>-8</v>
       </c>
-      <c r="E12" s="138">
+      <c r="E12" s="136">
         <v>-8</v>
       </c>
-      <c r="F12" s="136">
+      <c r="F12" s="134">
         <v>-4</v>
       </c>
-      <c r="G12" s="137">
+      <c r="G12" s="135">
         <v>-4</v>
       </c>
-      <c r="H12" s="137">
+      <c r="H12" s="135">
         <v>-4</v>
       </c>
-      <c r="I12" s="138">
+      <c r="I12" s="136">
         <v>-4</v>
       </c>
-      <c r="J12" s="136">
+      <c r="J12" s="134">
         <v>0</v>
       </c>
-      <c r="K12" s="137">
+      <c r="K12" s="135">
         <v>0</v>
       </c>
-      <c r="L12" s="137">
+      <c r="L12" s="135">
         <v>0</v>
       </c>
-      <c r="M12" s="138">
+      <c r="M12" s="136">
         <v>0</v>
       </c>
-      <c r="N12" s="136">
+      <c r="N12" s="134">
         <v>4</v>
       </c>
-      <c r="O12" s="142">
+      <c r="O12" s="140">
         <v>4</v>
       </c>
-      <c r="P12" s="142">
+      <c r="P12" s="140">
         <v>4</v>
       </c>
-      <c r="Q12" s="138">
+      <c r="Q12" s="136">
         <v>4</v>
       </c>
-      <c r="R12" s="136">
+      <c r="R12" s="134">
         <v>8</v>
       </c>
-      <c r="S12" s="142">
+      <c r="S12" s="140">
         <v>8</v>
       </c>
-      <c r="T12" s="142">
+      <c r="T12" s="140">
         <v>8</v>
       </c>
-      <c r="U12" s="138">
+      <c r="U12" s="136">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B13" s="139">
-        <f t="shared" ref="B13:H13" si="36">C13-1</f>
+      <c r="B13" s="137">
+        <f t="shared" ref="B13:H13" si="4">C13-1</f>
         <v>-8</v>
       </c>
-      <c r="C13" s="140">
-        <f t="shared" si="36"/>
+      <c r="C13" s="138">
+        <f t="shared" si="4"/>
         <v>-7</v>
       </c>
-      <c r="D13" s="140">
-        <f t="shared" si="36"/>
+      <c r="D13" s="138">
+        <f t="shared" si="4"/>
         <v>-6</v>
       </c>
-      <c r="E13" s="141">
-        <f t="shared" si="36"/>
+      <c r="E13" s="139">
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
-      <c r="F13" s="139">
-        <f t="shared" si="36"/>
+      <c r="F13" s="137">
+        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-      <c r="G13" s="140">
-        <f t="shared" si="36"/>
+      <c r="G13" s="138">
+        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
-      <c r="H13" s="140">
-        <f t="shared" si="36"/>
+      <c r="H13" s="138">
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
-      <c r="I13" s="141">
+      <c r="I13" s="139">
         <f>J13-1</f>
         <v>-1</v>
       </c>
-      <c r="J13" s="139">
+      <c r="J13" s="137">
         <v>0</v>
       </c>
-      <c r="K13" s="140">
+      <c r="K13" s="138">
         <f>J13+1</f>
         <v>1</v>
       </c>
-      <c r="L13" s="140">
-        <f t="shared" ref="L13:U13" si="37">K13+1</f>
+      <c r="L13" s="138">
+        <f t="shared" ref="L13:U13" si="5">K13+1</f>
         <v>2</v>
       </c>
-      <c r="M13" s="141">
-        <f t="shared" si="37"/>
+      <c r="M13" s="139">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="N13" s="139">
-        <f t="shared" si="37"/>
+      <c r="N13" s="137">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="O13" s="140">
-        <f t="shared" si="37"/>
+      <c r="O13" s="138">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="P13" s="140">
-        <f t="shared" si="37"/>
+      <c r="P13" s="138">
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="Q13" s="141">
-        <f t="shared" si="37"/>
+      <c r="Q13" s="139">
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="R13" s="139">
-        <f t="shared" si="37"/>
+      <c r="R13" s="137">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="S13" s="140">
-        <f t="shared" si="37"/>
+      <c r="S13" s="138">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="T13" s="140">
-        <f t="shared" si="37"/>
+      <c r="T13" s="138">
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="U13" s="141">
-        <f t="shared" si="37"/>
+      <c r="U13" s="139">
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D14" s="132"/>
-      <c r="E14" s="133"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="134"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="133"/>
-      <c r="J14" s="133"/>
-      <c r="K14" s="134"/>
-      <c r="L14" s="132"/>
-      <c r="M14" s="133"/>
-      <c r="N14" s="133"/>
-      <c r="O14" s="134"/>
-      <c r="P14" s="132"/>
-      <c r="Q14" s="133"/>
-      <c r="R14" s="133"/>
-      <c r="S14" s="134"/>
-      <c r="T14" s="132"/>
-      <c r="U14" s="133"/>
-      <c r="V14" s="133"/>
-      <c r="W14" s="134"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="132"/>
+      <c r="H14" s="130"/>
+      <c r="I14" s="131"/>
+      <c r="J14" s="131"/>
+      <c r="K14" s="132"/>
+      <c r="L14" s="130"/>
+      <c r="M14" s="131"/>
+      <c r="N14" s="131"/>
+      <c r="O14" s="132"/>
+      <c r="P14" s="130"/>
+      <c r="Q14" s="131"/>
+      <c r="R14" s="131"/>
+      <c r="S14" s="132"/>
+      <c r="T14" s="130"/>
+      <c r="U14" s="131"/>
+      <c r="V14" s="131"/>
+      <c r="W14" s="132"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D15" s="136"/>
-      <c r="E15" s="137"/>
-      <c r="F15" s="137"/>
-      <c r="G15" s="138"/>
-      <c r="H15" s="136"/>
-      <c r="I15" s="137"/>
-      <c r="J15" s="137"/>
-      <c r="K15" s="138"/>
-      <c r="L15" s="136"/>
-      <c r="M15" s="137"/>
-      <c r="N15" s="137"/>
-      <c r="O15" s="138"/>
-      <c r="P15" s="136"/>
-      <c r="Q15" s="137"/>
-      <c r="R15" s="137"/>
-      <c r="S15" s="138"/>
-      <c r="T15" s="136"/>
-      <c r="U15" s="137"/>
-      <c r="V15" s="137"/>
-      <c r="W15" s="138"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="135"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="136"/>
+      <c r="H15" s="134"/>
+      <c r="I15" s="135"/>
+      <c r="J15" s="135"/>
+      <c r="K15" s="136"/>
+      <c r="L15" s="134"/>
+      <c r="M15" s="135"/>
+      <c r="N15" s="135"/>
+      <c r="O15" s="136"/>
+      <c r="P15" s="134"/>
+      <c r="Q15" s="135"/>
+      <c r="R15" s="135"/>
+      <c r="S15" s="136"/>
+      <c r="T15" s="134"/>
+      <c r="U15" s="135"/>
+      <c r="V15" s="135"/>
+      <c r="W15" s="136"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D16" s="136"/>
-      <c r="E16" s="137"/>
-      <c r="F16" s="137"/>
-      <c r="G16" s="138"/>
-      <c r="H16" s="136"/>
-      <c r="I16" s="137"/>
-      <c r="J16" s="137"/>
-      <c r="K16" s="138"/>
-      <c r="L16" s="136"/>
-      <c r="M16" s="137"/>
-      <c r="N16" s="137"/>
-      <c r="O16" s="138"/>
-      <c r="P16" s="136"/>
-      <c r="Q16" s="137"/>
-      <c r="R16" s="137"/>
-      <c r="S16" s="138"/>
-      <c r="T16" s="136"/>
-      <c r="U16" s="137"/>
-      <c r="V16" s="137"/>
-      <c r="W16" s="138"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="135"/>
+      <c r="G16" s="136"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="135"/>
+      <c r="J16" s="135"/>
+      <c r="K16" s="136"/>
+      <c r="L16" s="134"/>
+      <c r="M16" s="135"/>
+      <c r="N16" s="135"/>
+      <c r="O16" s="136"/>
+      <c r="P16" s="134"/>
+      <c r="Q16" s="135"/>
+      <c r="R16" s="135"/>
+      <c r="S16" s="136"/>
+      <c r="T16" s="134"/>
+      <c r="U16" s="135"/>
+      <c r="V16" s="135"/>
+      <c r="W16" s="136"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="135">
-        <f t="shared" ref="B17:H17" si="38">C17-1</f>
+      <c r="B17" s="133">
+        <f t="shared" ref="B17:H17" si="6">C17-1</f>
         <v>-8</v>
       </c>
-      <c r="C17" s="135">
-        <f t="shared" si="38"/>
+      <c r="C17" s="133">
+        <f t="shared" si="6"/>
         <v>-7</v>
       </c>
-      <c r="D17" s="139">
-        <f t="shared" si="38"/>
+      <c r="D17" s="137">
+        <f t="shared" si="6"/>
         <v>-6</v>
       </c>
-      <c r="E17" s="140">
-        <f t="shared" si="38"/>
+      <c r="E17" s="138">
+        <f t="shared" si="6"/>
         <v>-5</v>
       </c>
-      <c r="F17" s="140">
-        <f t="shared" si="38"/>
+      <c r="F17" s="138">
+        <f t="shared" si="6"/>
         <v>-4</v>
       </c>
-      <c r="G17" s="141">
-        <f t="shared" si="38"/>
+      <c r="G17" s="139">
+        <f t="shared" si="6"/>
         <v>-3</v>
       </c>
-      <c r="H17" s="139">
-        <f t="shared" si="38"/>
+      <c r="H17" s="137">
+        <f t="shared" si="6"/>
         <v>-2</v>
       </c>
-      <c r="I17" s="140">
+      <c r="I17" s="138">
         <f>J17-1</f>
         <v>-1</v>
       </c>
-      <c r="J17" s="140">
+      <c r="J17" s="138">
         <v>0</v>
       </c>
-      <c r="K17" s="141">
+      <c r="K17" s="139">
         <f>J17+1</f>
         <v>1</v>
       </c>
-      <c r="L17" s="139">
-        <f t="shared" ref="L17:U17" si="39">K17+1</f>
+      <c r="L17" s="137">
+        <f t="shared" ref="L17:U17" si="7">K17+1</f>
         <v>2</v>
       </c>
-      <c r="M17" s="140">
-        <f t="shared" si="39"/>
+      <c r="M17" s="138">
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="N17" s="140">
-        <f t="shared" si="39"/>
+      <c r="N17" s="138">
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="O17" s="141">
-        <f t="shared" si="39"/>
+      <c r="O17" s="139">
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="P17" s="139">
-        <f t="shared" si="39"/>
+      <c r="P17" s="137">
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="Q17" s="140">
-        <f t="shared" si="39"/>
+      <c r="Q17" s="138">
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="R17" s="140">
-        <f t="shared" si="39"/>
+      <c r="R17" s="138">
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="S17" s="141">
-        <f t="shared" si="39"/>
+      <c r="S17" s="139">
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="T17" s="139">
-        <f t="shared" si="39"/>
+      <c r="T17" s="137">
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="U17" s="140">
-        <f t="shared" si="39"/>
+      <c r="U17" s="138">
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
-      <c r="V17" s="140"/>
-      <c r="W17" s="141"/>
+      <c r="V17" s="138"/>
+      <c r="W17" s="139"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="132"/>
-      <c r="C18" s="133"/>
-      <c r="D18" s="133"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="132"/>
-      <c r="G18" s="133"/>
-      <c r="H18" s="133"/>
-      <c r="I18" s="134"/>
-      <c r="J18" s="132"/>
-      <c r="K18" s="133"/>
-      <c r="L18" s="133"/>
-      <c r="M18" s="134"/>
-      <c r="N18" s="132"/>
-      <c r="O18" s="133"/>
-      <c r="P18" s="133"/>
-      <c r="Q18" s="134"/>
-      <c r="R18" s="132"/>
-      <c r="S18" s="133"/>
-      <c r="T18" s="133"/>
-      <c r="U18" s="134"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="131"/>
+      <c r="D18" s="131"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="131"/>
+      <c r="H18" s="131"/>
+      <c r="I18" s="132"/>
+      <c r="J18" s="130"/>
+      <c r="K18" s="131"/>
+      <c r="L18" s="131"/>
+      <c r="M18" s="132"/>
+      <c r="N18" s="130"/>
+      <c r="O18" s="131"/>
+      <c r="P18" s="131"/>
+      <c r="Q18" s="132"/>
+      <c r="R18" s="130"/>
+      <c r="S18" s="131"/>
+      <c r="T18" s="131"/>
+      <c r="U18" s="132"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="136"/>
-      <c r="C19" s="137"/>
-      <c r="D19" s="137"/>
-      <c r="E19" s="138"/>
-      <c r="F19" s="136"/>
-      <c r="G19" s="137"/>
-      <c r="H19" s="137"/>
-      <c r="I19" s="138"/>
-      <c r="J19" s="136"/>
-      <c r="K19" s="137"/>
-      <c r="L19" s="137"/>
-      <c r="M19" s="138"/>
-      <c r="N19" s="136"/>
-      <c r="O19" s="137"/>
-      <c r="P19" s="137"/>
-      <c r="Q19" s="138"/>
-      <c r="R19" s="136"/>
-      <c r="S19" s="137"/>
-      <c r="T19" s="137"/>
-      <c r="U19" s="138"/>
+      <c r="B19" s="134"/>
+      <c r="C19" s="135"/>
+      <c r="D19" s="135"/>
+      <c r="E19" s="136"/>
+      <c r="F19" s="134"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="135"/>
+      <c r="I19" s="136"/>
+      <c r="J19" s="134"/>
+      <c r="K19" s="135"/>
+      <c r="L19" s="135"/>
+      <c r="M19" s="136"/>
+      <c r="N19" s="134"/>
+      <c r="O19" s="135"/>
+      <c r="P19" s="135"/>
+      <c r="Q19" s="136"/>
+      <c r="R19" s="134"/>
+      <c r="S19" s="135"/>
+      <c r="T19" s="135"/>
+      <c r="U19" s="136"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="136"/>
-      <c r="C20" s="137"/>
-      <c r="D20" s="137"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="136"/>
-      <c r="G20" s="137"/>
-      <c r="H20" s="137"/>
-      <c r="I20" s="138"/>
-      <c r="J20" s="136"/>
-      <c r="K20" s="137"/>
-      <c r="L20" s="137"/>
-      <c r="M20" s="138"/>
-      <c r="N20" s="136"/>
-      <c r="O20" s="137"/>
-      <c r="P20" s="137"/>
-      <c r="Q20" s="138"/>
-      <c r="R20" s="136"/>
-      <c r="S20" s="137"/>
-      <c r="T20" s="137"/>
-      <c r="U20" s="138"/>
+      <c r="B20" s="134"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="135"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="134"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="135"/>
+      <c r="I20" s="136"/>
+      <c r="J20" s="134"/>
+      <c r="K20" s="135"/>
+      <c r="L20" s="135"/>
+      <c r="M20" s="136"/>
+      <c r="N20" s="134"/>
+      <c r="O20" s="135"/>
+      <c r="P20" s="135"/>
+      <c r="Q20" s="136"/>
+      <c r="R20" s="134"/>
+      <c r="S20" s="135"/>
+      <c r="T20" s="135"/>
+      <c r="U20" s="136"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="139"/>
-      <c r="C21" s="140"/>
-      <c r="D21" s="140"/>
-      <c r="E21" s="141"/>
-      <c r="F21" s="139"/>
-      <c r="G21" s="140"/>
-      <c r="H21" s="140"/>
-      <c r="I21" s="141"/>
-      <c r="J21" s="139"/>
-      <c r="K21" s="140"/>
-      <c r="L21" s="140"/>
-      <c r="M21" s="141"/>
-      <c r="N21" s="139"/>
-      <c r="O21" s="140"/>
-      <c r="P21" s="140"/>
-      <c r="Q21" s="141"/>
-      <c r="R21" s="139"/>
-      <c r="S21" s="140"/>
-      <c r="T21" s="140"/>
-      <c r="U21" s="141"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="138"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="137"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="138"/>
+      <c r="I21" s="139"/>
+      <c r="J21" s="137"/>
+      <c r="K21" s="138"/>
+      <c r="L21" s="138"/>
+      <c r="M21" s="139"/>
+      <c r="N21" s="137"/>
+      <c r="O21" s="138"/>
+      <c r="P21" s="138"/>
+      <c r="Q21" s="139"/>
+      <c r="R21" s="137"/>
+      <c r="S21" s="138"/>
+      <c r="T21" s="138"/>
+      <c r="U21" s="139"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C65" si="0">B2*range</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>TRUNC(C2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>TRUNC(C2+0.5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B19" si="1">B2+incer</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="2">TRUNC(C3)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E22" si="3">TRUNC(C3+0.5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1.2750000000000001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>2.125</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2.9749999999999996</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>3.8249999999999997</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>4.2499999999999991</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>4.6749999999999998</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>5.5250000000000004</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>5.95</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>6.3750000000000009</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>6.8000000000000016</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>0.4250000000000001</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>7.2250000000000014</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <f t="shared" ref="B20:B24" si="4">B19+incer</f>
+        <v>0.45000000000000012</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>7.6500000000000021</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <f t="shared" si="4"/>
+        <v>0.47500000000000014</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>8.0750000000000028</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <f t="shared" si="4"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>8.5000000000000018</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <f t="shared" ref="B23:B68" si="5">B22+incer</f>
+        <v>0.52500000000000013</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>8.9250000000000025</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:E68" si="6">TRUNC(C23+0.5)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <f t="shared" si="5"/>
+        <v>0.55000000000000016</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>9.3500000000000032</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <f t="shared" si="5"/>
+        <v>0.57500000000000018</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>9.7750000000000021</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <f t="shared" si="5"/>
+        <v>0.6000000000000002</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>10.200000000000003</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <f t="shared" si="5"/>
+        <v>0.62500000000000022</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>10.625000000000004</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <f t="shared" si="5"/>
+        <v>0.65000000000000024</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>11.050000000000004</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <f t="shared" si="5"/>
+        <v>0.67500000000000027</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>11.475000000000005</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <f t="shared" si="5"/>
+        <v>0.70000000000000029</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>11.900000000000006</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <f t="shared" si="5"/>
+        <v>0.72500000000000031</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>12.325000000000005</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <f t="shared" si="5"/>
+        <v>0.75000000000000033</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>12.750000000000005</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <f t="shared" si="5"/>
+        <v>0.77500000000000036</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>13.175000000000006</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <f t="shared" si="5"/>
+        <v>0.80000000000000038</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>13.600000000000007</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <f t="shared" si="5"/>
+        <v>0.8250000000000004</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>14.025000000000007</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <f t="shared" si="5"/>
+        <v>0.85000000000000042</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>14.450000000000006</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <f t="shared" si="5"/>
+        <v>0.87500000000000044</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>14.875000000000007</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <f t="shared" si="5"/>
+        <v>0.90000000000000047</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>15.300000000000008</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <f t="shared" si="5"/>
+        <v>0.92500000000000049</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>15.725000000000009</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <f t="shared" si="5"/>
+        <v>0.95000000000000051</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>16.150000000000009</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f t="shared" si="5"/>
+        <v>0.97500000000000053</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>16.57500000000001</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>17.000000000000007</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <f t="shared" si="5"/>
+        <v>1.0250000000000004</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>17.425000000000004</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <f t="shared" si="5"/>
+        <v>1.0500000000000003</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>17.850000000000005</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <f t="shared" si="5"/>
+        <v>1.0750000000000002</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>18.275000000000002</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <f t="shared" si="5"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>18.700000000000003</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <f t="shared" si="5"/>
+        <v>1.125</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>19.125</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <f t="shared" si="5"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>19.549999999999997</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <f t="shared" si="5"/>
+        <v>1.1749999999999998</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>19.974999999999998</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <f t="shared" si="5"/>
+        <v>1.1999999999999997</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>20.399999999999995</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <f t="shared" si="5"/>
+        <v>1.2249999999999996</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>20.824999999999996</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <f t="shared" si="5"/>
+        <v>1.2499999999999996</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>21.249999999999993</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <f t="shared" si="5"/>
+        <v>1.2749999999999995</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>21.67499999999999</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <f t="shared" si="5"/>
+        <v>1.2999999999999994</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>22.099999999999991</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <f t="shared" si="5"/>
+        <v>1.3249999999999993</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>22.524999999999988</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <f t="shared" si="5"/>
+        <v>1.3499999999999992</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>22.949999999999985</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <f t="shared" si="5"/>
+        <v>1.3749999999999991</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>23.374999999999986</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <f t="shared" si="5"/>
+        <v>1.399999999999999</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>23.799999999999983</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <f t="shared" si="5"/>
+        <v>1.4249999999999989</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>24.22499999999998</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <f t="shared" si="5"/>
+        <v>1.4499999999999988</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>24.649999999999981</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <f t="shared" si="5"/>
+        <v>1.4749999999999988</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>25.074999999999978</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <f t="shared" si="5"/>
+        <v>1.4999999999999987</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>25.499999999999979</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="6"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <f t="shared" si="5"/>
+        <v>1.5249999999999986</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>25.924999999999976</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="6"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <f t="shared" si="5"/>
+        <v>1.5499999999999985</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>26.349999999999973</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="6"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <f t="shared" si="5"/>
+        <v>1.5749999999999984</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>26.774999999999974</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="6"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <f t="shared" si="5"/>
+        <v>1.5999999999999983</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ref="C66:C68" si="7">B66*range</f>
+        <v>27.199999999999971</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="6"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <f t="shared" si="5"/>
+        <v>1.6249999999999982</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="7"/>
+        <v>27.624999999999972</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D68" si="8">TRUNC(C67)</f>
+        <v>27</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <f t="shared" si="5"/>
+        <v>1.6499999999999981</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="7"/>
+        <v>28.049999999999969</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -55433,7 +56662,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <f t="shared" ref="D19:Q35" si="6">IF(ISODD($C19),D$2,D$2+$B$1)</f>
+        <f t="shared" ref="D19:D35" si="6">IF(ISODD($C19),D$2,D$2+$B$1)</f>
         <v>0</v>
       </c>
       <c r="E19">
@@ -56331,7 +57560,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f t="shared" ref="A32:A35" si="8">+A31+1</f>
+        <f>+A31+1</f>
         <v>13</v>
       </c>
       <c r="B32">
@@ -56401,7 +57630,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f t="shared" si="8"/>
+        <f>+A32+1</f>
         <v>14</v>
       </c>
       <c r="B33">
@@ -56471,7 +57700,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34">
-        <f t="shared" si="8"/>
+        <f>+A33+1</f>
         <v>15</v>
       </c>
       <c r="B34">
@@ -56541,7 +57770,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f t="shared" si="8"/>
+        <f>+A34+1</f>
         <v>16</v>
       </c>
       <c r="B35">
@@ -56557,55 +57786,55 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="E35:Q35" si="8">IF(ISODD($C35),E$2,E$2+$B$1)</f>
         <v>-6</v>
       </c>
       <c r="F35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-2</v>
       </c>
       <c r="G35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-2</v>
       </c>
       <c r="H35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-2</v>
       </c>
       <c r="I35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-2</v>
       </c>
       <c r="J35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="K35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="L35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="M35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="N35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="O35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="P35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
     </row>

</xml_diff>